<commit_message>
GH ACTION Autorun Sat Jul 31 23:39:38 UTC 2021
</commit_message>
<xml_diff>
--- a/data/graph-data/arrow_plot.xlsx
+++ b/data/graph-data/arrow_plot.xlsx
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D22">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GH ACTION Autorun Sun Aug  1 06:11:00 UTC 2021
</commit_message>
<xml_diff>
--- a/data/graph-data/arrow_plot.xlsx
+++ b/data/graph-data/arrow_plot.xlsx
@@ -428,7 +428,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="D4">
         <v>0.48</v>
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="D8">
         <v>0.78</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Sun Aug  1 18:10:07 UTC 2021
</commit_message>
<xml_diff>
--- a/data/graph-data/arrow_plot.xlsx
+++ b/data/graph-data/arrow_plot.xlsx
@@ -388,7 +388,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -396,15 +396,15 @@
         </is>
       </c>
       <c r="C2">
+        <v>0.37</v>
+      </c>
+      <c r="D2">
         <v>0.39</v>
-      </c>
-      <c r="D2">
-        <v>0.37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -412,15 +412,15 @@
         </is>
       </c>
       <c r="C3">
+        <v>0.39</v>
+      </c>
+      <c r="D3">
         <v>0.36</v>
-      </c>
-      <c r="D3">
-        <v>0.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -428,15 +428,15 @@
         </is>
       </c>
       <c r="C4">
+        <v>0.49</v>
+      </c>
+      <c r="D4">
         <v>0.47</v>
-      </c>
-      <c r="D4">
-        <v>0.48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -444,15 +444,15 @@
         </is>
       </c>
       <c r="C5">
+        <v>0.37</v>
+      </c>
+      <c r="D5">
         <v>0.36</v>
-      </c>
-      <c r="D5">
-        <v>0.34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -463,12 +463,12 @@
         <v>0.77</v>
       </c>
       <c r="D6">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -476,31 +476,28 @@
         </is>
       </c>
       <c r="C7">
+        <v>0.41</v>
+      </c>
+      <c r="D7">
         <v>0.4</v>
-      </c>
-      <c r="D7">
-        <v>0.39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Lazio</t>
         </is>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.74</v>
-      </c>
-      <c r="D8">
-        <v>0.78</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -508,15 +505,15 @@
         </is>
       </c>
       <c r="C9">
+        <v>0.61</v>
+      </c>
+      <c r="D9">
         <v>0.5600000000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -527,12 +524,12 @@
         <v>0.38</v>
       </c>
       <c r="D10">
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -540,15 +537,15 @@
         </is>
       </c>
       <c r="C11">
+        <v>0.52</v>
+      </c>
+      <c r="D11">
         <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>0.46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -556,7 +553,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="D12">
         <v>0.17</v>
@@ -564,7 +561,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -572,31 +569,28 @@
         </is>
       </c>
       <c r="C13">
+        <v>0.33</v>
+      </c>
+      <c r="D13">
         <v>0.34</v>
-      </c>
-      <c r="D13">
-        <v>0.32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>P.A. Trento</t>
         </is>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.45</v>
-      </c>
-      <c r="D14">
-        <v>0.46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -604,15 +598,15 @@
         </is>
       </c>
       <c r="C15">
+        <v>0.31</v>
+      </c>
+      <c r="D15">
         <v>0.3</v>
-      </c>
-      <c r="D15">
-        <v>0.29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -623,12 +617,12 @@
         <v>0.27</v>
       </c>
       <c r="D16">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -639,12 +633,12 @@
         <v>1.39</v>
       </c>
       <c r="D17">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -652,15 +646,15 @@
         </is>
       </c>
       <c r="C18">
+        <v>0.97</v>
+      </c>
+      <c r="D18">
         <v>0.96</v>
-      </c>
-      <c r="D18">
-        <v>0.91</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -668,15 +662,15 @@
         </is>
       </c>
       <c r="C19">
+        <v>1.17</v>
+      </c>
+      <c r="D19">
         <v>1.11</v>
-      </c>
-      <c r="D19">
-        <v>1.07</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -684,15 +678,15 @@
         </is>
       </c>
       <c r="C20">
+        <v>0.83</v>
+      </c>
+      <c r="D20">
         <v>0.86</v>
-      </c>
-      <c r="D20">
-        <v>0.84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -700,15 +694,15 @@
         </is>
       </c>
       <c r="C21">
+        <v>0.22</v>
+      </c>
+      <c r="D21">
         <v>0.23</v>
-      </c>
-      <c r="D21">
-        <v>0.25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -716,10 +710,10 @@
         </is>
       </c>
       <c r="C22">
+        <v>0.93</v>
+      </c>
+      <c r="D22">
         <v>0.9399999999999999</v>
-      </c>
-      <c r="D22">
-        <v>0.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>